<commit_message>
Update results for exercise 5
</commit_message>
<xml_diff>
--- a/ex05/BRTT result spreadsheet.xlsx
+++ b/ex05/BRTT result spreadsheet.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="24">
   <si>
     <t xml:space="preserve">Test name:</t>
   </si>
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t xml:space="preserve">Select scale (in us):</t>
-  </si>
-  <si>
-    <t xml:space="preserve">git </t>
   </si>
 </sst>
 </file>
@@ -314,7 +311,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -368,7 +365,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Calculations!$E$5</c:f>
+              <c:f>Calculations!$O$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -468,72 +465,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Calculations!$E$10:$E$30</c:f>
+              <c:f>Calculations!$O$10:$O$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>970</c:v>
+                  <c:v>517</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -544,7 +541,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Calculations!$F$5</c:f>
+              <c:f>Calculations!$P$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -644,72 +641,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Calculations!$F$10:$F$30</c:f>
+              <c:f>Calculations!$P$10:$P$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>961</c:v>
+                  <c:v>533</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6</c:v>
+                  <c:v>433</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -720,7 +717,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Calculations!$G$5</c:f>
+              <c:f>Calculations!$Q$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -820,21 +817,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Calculations!$G$10:$G$30</c:f>
+              <c:f>Calculations!$Q$10:$Q$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>967</c:v>
+                  <c:v>524</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -843,49 +840,49 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="16">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7</c:v>
+                  <c:v>443</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -893,11 +890,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="43093354"/>
-        <c:axId val="82398244"/>
+        <c:axId val="99578860"/>
+        <c:axId val="56835047"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="43093354"/>
+        <c:axId val="99578860"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -971,14 +968,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82398244"/>
+        <c:crossAx val="56835047"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82398244"/>
+        <c:axId val="56835047"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1062,7 +1059,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43093354"/>
+        <c:crossAx val="99578860"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1099,7 +1096,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1153,7 +1150,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Calculations!$J$5</c:f>
+              <c:f>Calculations!$T$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1253,51 +1250,51 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Calculations!$J$10:$J$30</c:f>
+              <c:f>Calculations!$T$10:$T$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>995</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -1329,7 +1326,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Calculations!$K$5</c:f>
+              <c:f>Calculations!$U$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1429,51 +1426,51 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Calculations!$K$10:$K$30</c:f>
+              <c:f>Calculations!$U$10:$U$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>992</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -1505,7 +1502,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Calculations!$L$5</c:f>
+              <c:f>Calculations!$V$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1605,54 +1602,54 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Calculations!$L$10:$L$30</c:f>
+              <c:f>Calculations!$V$10:$V$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>988</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -1670,7 +1667,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1678,11 +1675,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="5572311"/>
-        <c:axId val="34023281"/>
+        <c:axId val="88483314"/>
+        <c:axId val="68134101"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="5572311"/>
+        <c:axId val="88483314"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1756,14 +1753,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34023281"/>
+        <c:crossAx val="68134101"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="34023281"/>
+        <c:axId val="68134101"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1847,7 +1844,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5572311"/>
+        <c:crossAx val="88483314"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1884,7 +1881,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1938,7 +1935,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Calculations!$O$5</c:f>
+              <c:f>Calculations!$Y$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2038,72 +2035,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Calculations!$O$10:$O$30</c:f>
+              <c:f>Calculations!$Y$10:$Y$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>517</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="15">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>450</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2114,7 +2111,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Calculations!$P$5</c:f>
+              <c:f>Calculations!$Z$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2214,72 +2211,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Calculations!$P$10:$P$30</c:f>
+              <c:f>Calculations!$Z$10:$Z$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>533</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>433</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2290,7 +2287,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Calculations!$Q$5</c:f>
+              <c:f>Calculations!$AA$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2390,60 +2387,60 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Calculations!$Q$10:$Q$30</c:f>
+              <c:f>Calculations!$AA$10:$AA$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>524</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
@@ -2452,10 +2449,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>443</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2463,11 +2460,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="16675379"/>
-        <c:axId val="34985081"/>
+        <c:axId val="49914605"/>
+        <c:axId val="92047471"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="16675379"/>
+        <c:axId val="49914605"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2541,14 +2538,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34985081"/>
+        <c:crossAx val="92047471"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="34985081"/>
+        <c:axId val="92047471"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2632,7 +2629,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16675379"/>
+        <c:crossAx val="49914605"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2669,7 +2666,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2723,7 +2720,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Calculations!$T$5</c:f>
+              <c:f>Calculations!$AD$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2823,72 +2820,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Calculations!$T$10:$T$30</c:f>
+              <c:f>Calculations!$AD$10:$AD$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>65</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>66</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>62</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>73</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>90</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>74</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>82</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>85</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>57</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>61</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>77</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>80</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>72</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2899,7 +2896,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Calculations!$U$5</c:f>
+              <c:f>Calculations!$AE$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2999,72 +2996,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Calculations!$U$10:$U$30</c:f>
+              <c:f>Calculations!$AE$10:$AE$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>62</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>63</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>58</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>61</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>73</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>83</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>71</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>92</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>63</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>56</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>76</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>79</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>82</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3075,7 +3072,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Calculations!$V$5</c:f>
+              <c:f>Calculations!$AF$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3175,72 +3172,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Calculations!$V$10:$V$30</c:f>
+              <c:f>Calculations!$AF$10:$AF$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>54</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>69</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>66</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>86</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>73</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>81</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>66</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>61</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>73</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>79</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>82</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3248,11 +3245,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="52212871"/>
-        <c:axId val="66008970"/>
+        <c:axId val="86828305"/>
+        <c:axId val="25899069"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="52212871"/>
+        <c:axId val="86828305"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3326,14 +3323,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66008970"/>
+        <c:crossAx val="25899069"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66008970"/>
+        <c:axId val="25899069"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3417,7 +3414,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52212871"/>
+        <c:crossAx val="86828305"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3454,7 +3451,1205 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Calculations!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Task A (w/ 5us delay)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4f81bd"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Calculations!$D$10:$D$30</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>675</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>825</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>975</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1125</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1275</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1425</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Calculations!$H$10:$H$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>2898</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Calculations!$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Task B (CPU0 w/o disturbance)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="c0504d"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Calculations!$D$10:$D$30</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>675</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>825</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>975</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1125</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1275</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1425</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Calculations!$M$10:$M$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>2975</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Calculations!$O$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Task C (CPU0 w/ disturbance)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="9bbb59"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Calculations!$D$10:$D$30</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>675</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>825</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>975</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1125</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1275</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1425</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Calculations!$R$10:$R$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1574</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1326</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Calculations!$T$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Task D (1ms CPU0 w/o disturbance)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="8064a2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Calculations!$D$10:$D$30</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>675</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>825</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>975</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1125</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1275</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1425</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Calculations!$W$10:$W$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>259</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>266</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>238</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Calculations!$Y$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Task D (1ms CPU0 w/ disturbance)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4bacc6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Calculations!$D$10:$D$30</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>675</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>825</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>975</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1125</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1275</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1425</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Calculations!$AB$10:$AB$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>231</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Calculations!$AD$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>…</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="f79646"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Calculations!$D$10:$D$30</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>675</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>825</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>975</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1125</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1275</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1425</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Calculations!$AG$10:$AG$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="150"/>
+        <c:overlap val="0"/>
+        <c:axId val="35224184"/>
+        <c:axId val="75610516"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="35224184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="878787"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="75610516"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="75610516"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="878787"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="878787"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="35224184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3508,7 +4703,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Calculations!$Y$5</c:f>
+              <c:f>Calculations!$E$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3608,57 +4803,57 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Calculations!$Y$10:$Y$30</c:f>
+              <c:f>Calculations!$E$10:$E$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>69</c:v>
+                  <c:v>970</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>81</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>82</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>62</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>88</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>69</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>72</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>58</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>70</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>64</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>60</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
@@ -3684,7 +4879,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Calculations!$Z$5</c:f>
+              <c:f>Calculations!$F$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3784,57 +4979,57 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Calculations!$Z$10:$Z$30</c:f>
+              <c:f>Calculations!$F$10:$F$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>59</c:v>
+                  <c:v>961</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>67</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>71</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>80</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>81</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>72</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>69</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>72</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>60</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>69</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>64</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
@@ -3843,13 +5038,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="20">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3860,7 +5055,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Calculations!$AA$5</c:f>
+              <c:f>Calculations!$G$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3960,72 +5155,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Calculations!$AA$10:$AA$30</c:f>
+              <c:f>Calculations!$G$10:$G$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>57</c:v>
+                  <c:v>967</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>73</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>88</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>83</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>74</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>73</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>61</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>67</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>62</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="20">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4033,11 +5228,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="42109651"/>
-        <c:axId val="64790311"/>
+        <c:axId val="36063903"/>
+        <c:axId val="64285951"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="42109651"/>
+        <c:axId val="36063903"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4111,14 +5306,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64790311"/>
+        <c:crossAx val="64285951"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64790311"/>
+        <c:axId val="64285951"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4202,7 +5397,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42109651"/>
+        <c:crossAx val="36063903"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4239,7 +5434,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4293,7 +5488,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Calculations!$AD$5</c:f>
+              <c:f>Calculations!$J$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4393,72 +5588,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Calculations!$AD$10:$AD$30</c:f>
+              <c:f>Calculations!$J$10:$J$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v/>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4469,7 +5664,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Calculations!$AE$5</c:f>
+              <c:f>Calculations!$K$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4569,72 +5764,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Calculations!$AE$10:$AE$30</c:f>
+              <c:f>Calculations!$K$10:$K$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>992</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4645,7 +5840,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Calculations!$AF$5</c:f>
+              <c:f>Calculations!$L$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4745,72 +5940,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Calculations!$AF$10:$AF$30</c:f>
+              <c:f>Calculations!$L$10:$L$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>988</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v/>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4818,11 +6013,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="68387190"/>
-        <c:axId val="32709029"/>
+        <c:axId val="65251591"/>
+        <c:axId val="65040363"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="68387190"/>
+        <c:axId val="65251591"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4896,14 +6091,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32709029"/>
+        <c:crossAx val="65040363"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="32709029"/>
+        <c:axId val="65040363"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4987,1205 +6182,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68387190"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:plotArea>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Calculations!$E$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Task A (w/ 5us delay)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4f81bd"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Calculations!$D$10:$D$30</c:f>
-              <c:strCache>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>225</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>375</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>450</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>525</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>600</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>675</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>750</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>825</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>975</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1050</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1125</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1200</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1275</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1350</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1425</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1500</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Calculations!$H$10:$H$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>2898</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Calculations!$J$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Task B (CPU0 w/o disturbance)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="c0504d"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Calculations!$D$10:$D$30</c:f>
-              <c:strCache>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>225</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>375</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>450</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>525</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>600</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>675</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>750</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>825</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>975</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1050</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1125</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1200</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1275</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1350</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1425</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1500</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Calculations!$M$10:$M$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>2975</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Calculations!$O$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Task C (CPU0 w/ disturbance)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="9bbb59"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Calculations!$D$10:$D$30</c:f>
-              <c:strCache>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>225</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>375</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>450</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>525</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>600</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>675</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>750</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>825</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>975</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1050</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1125</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1200</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1275</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1350</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1425</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1500</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Calculations!$R$10:$R$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>1574</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1326</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Calculations!$T$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Task D (1ms CPU0 w/o disturbance)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="8064a2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Calculations!$D$10:$D$30</c:f>
-              <c:strCache>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>225</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>375</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>450</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>525</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>600</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>675</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>750</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>825</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>975</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1050</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1125</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1200</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1275</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1350</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1425</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1500</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Calculations!$W$10:$W$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>181</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>198</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>174</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>179</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>212</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>259</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>218</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>243</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>266</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>186</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>178</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>226</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>238</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>236</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Calculations!$Y$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Task D (1ms CPU0 w/ disturbance)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4bacc6"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Calculations!$D$10:$D$30</c:f>
-              <c:strCache>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>225</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>375</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>450</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>525</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>600</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>675</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>750</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>825</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>975</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1050</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1125</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1200</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1275</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1350</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1425</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1500</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Calculations!$AB$10:$AB$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>185</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>215</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>219</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>231</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>251</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>203</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>251</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>212</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>217</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>179</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>203</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>195</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>187</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>24</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Calculations!$AD$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>…</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="f79646"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Calculations!$D$10:$D$30</c:f>
-              <c:strCache>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>225</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>375</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>450</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>525</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>600</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>675</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>750</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>825</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>975</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1050</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1125</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1200</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1275</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1350</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1425</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1500</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Calculations!$AG$10:$AG$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:gapWidth val="150"/>
-        <c:overlap val="0"/>
-        <c:axId val="92874850"/>
-        <c:axId val="58381089"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="92874850"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="878787"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="58381089"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="58381089"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="878787"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="878787"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="92874850"/>
+        <c:crossAx val="65251591"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -71167,7 +71164,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:T46"/>
+  <dimension ref="B1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="T46" activeCellId="0" sqref="T46"/>
@@ -71185,11 +71182,6 @@
       </c>
       <c r="D2" s="4" t="n">
         <v>1500</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T46" s="0" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>